<commit_message>
updating improved water classification based on 2017 WHO/UNICEF guidelines
</commit_message>
<xml_diff>
--- a/AssetSurveyItems_Match.xlsx
+++ b/AssetSurveyItems_Match.xlsx
@@ -1,19 +1,20 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11011"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11113"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://mcgill.sharepoint.com/sites/PROSPERED_Group/Shared Documents/General/CIHR RSBY India/data/Linking code and CSVs/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="29" documentId="8_{F77C4B80-A99E-7F40-A288-258E5FEBB2B2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{7D926B75-DE62-D845-B523-0A43FED8E1B3}"/>
+  <xr:revisionPtr revIDLastSave="97" documentId="8_{F77C4B80-A99E-7F40-A288-258E5FEBB2B2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{24427BF8-F743-1A4B-B820-01594330A9B0}"/>
   <bookViews>
-    <workbookView xWindow="2900" yWindow="500" windowWidth="20480" windowHeight="16520" xr2:uid="{87D403AE-B090-804E-AAD5-1AA8BD4EAB0C}"/>
+    <workbookView xWindow="13800" yWindow="500" windowWidth="20480" windowHeight="16520" activeTab="1" xr2:uid="{87D403AE-B090-804E-AAD5-1AA8BD4EAB0C}"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="Across Survyes" sheetId="1" r:id="rId1"/>
+    <sheet name="Correct order for AI" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="181029"/>
   <extLst>
@@ -36,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="725" uniqueCount="547">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="775" uniqueCount="577">
   <si>
     <t>DLHS3</t>
   </si>
@@ -1677,6 +1678,96 @@
   </si>
   <si>
     <t>NFHS5</t>
+  </si>
+  <si>
+    <t xml:space="preserve">  1   piped-water-into-dwelling-yardplot</t>
+  </si>
+  <si>
+    <t xml:space="preserve">           2   public-tap-stand-pipe</t>
+  </si>
+  <si>
+    <t xml:space="preserve">           3  tubewell-or-borehole</t>
+  </si>
+  <si>
+    <t xml:space="preserve">           4   protected-dugwell</t>
+  </si>
+  <si>
+    <t xml:space="preserve">           5   unprotected-dug-well</t>
+  </si>
+  <si>
+    <t>6 tanker/truck/cart</t>
+  </si>
+  <si>
+    <t>7other source</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 2   public-tap-stand-pipe</t>
+  </si>
+  <si>
+    <t>3  tubewell-or-borehole</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 1   piped-water-into-dwelling-yardplot</t>
+  </si>
+  <si>
+    <t>0 OPEN DEFECATION/NO FACILITY/OPEN SPACE OR FIELD</t>
+  </si>
+  <si>
+    <t xml:space="preserve">1 pour/flush latrine: connected to piped sewer system </t>
+  </si>
+  <si>
+    <t xml:space="preserve">2 pour/flush latrine: connected to septic tank </t>
+  </si>
+  <si>
+    <t xml:space="preserve">3 pour/flush latrine: connected to pit latrine </t>
+  </si>
+  <si>
+    <t xml:space="preserve">4 pour/flush latrine: connected to something else </t>
+  </si>
+  <si>
+    <t xml:space="preserve">5 pit latrine: ventilated improved pit </t>
+  </si>
+  <si>
+    <t xml:space="preserve">6 pit latrine: with slab </t>
+  </si>
+  <si>
+    <t xml:space="preserve">7 pit latrine: open or without slab </t>
+  </si>
+  <si>
+    <t>8 service latrine /dry toilet</t>
+  </si>
+  <si>
+    <t>9 OTHER</t>
+  </si>
+  <si>
+    <t>9 OPEN DEFECATION/NO FACILITY/OPEN SPACE OR FIELD</t>
+  </si>
+  <si>
+    <t>1 Electricity</t>
+  </si>
+  <si>
+    <t>2 LPG/ Natural Gas</t>
+  </si>
+  <si>
+    <t>3 Biogas</t>
+  </si>
+  <si>
+    <t>4 Kerosene</t>
+  </si>
+  <si>
+    <t>5 Coal / Ignite / Charcoal</t>
+  </si>
+  <si>
+    <t>6 Wood</t>
+  </si>
+  <si>
+    <t>7 Straw / Shrubs / Grass / Agricultural Crop Waste</t>
+  </si>
+  <si>
+    <t>8 Dung Cakes</t>
+  </si>
+  <si>
+    <t>96 Other</t>
   </si>
 </sst>
 </file>
@@ -1733,7 +1824,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="1">
+  <borders count="3">
     <border>
       <left/>
       <right/>
@@ -1741,22 +1832,53 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="9">
+  <cellXfs count="14">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1772,6 +1894,10 @@
     </ext>
   </extLst>
 </styleSheet>
+</file>
+
+<file path=xl/persons/person.xml><?xml version="1.0" encoding="utf-8"?>
+<personList xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -2073,7 +2199,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{55E3B49A-77A0-AD4A-81B0-B8BFD615B07C}">
   <dimension ref="A1:S132"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="I1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+    <sheetView topLeftCell="I1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A38" activePane="bottomLeft" state="frozen"/>
       <selection activeCell="D1" sqref="D1"/>
       <selection pane="bottomLeft" activeCell="I59" sqref="I59:J59"/>
@@ -2092,26 +2218,26 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:18" x14ac:dyDescent="0.2">
-      <c r="A1" s="6" t="s">
+      <c r="A1" s="7" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="6"/>
-      <c r="C1" s="6" t="s">
+      <c r="B1" s="7"/>
+      <c r="C1" s="7" t="s">
         <v>121</v>
       </c>
-      <c r="D1" s="6"/>
-      <c r="E1" s="6" t="s">
+      <c r="D1" s="7"/>
+      <c r="E1" s="7" t="s">
         <v>470</v>
       </c>
-      <c r="F1" s="6"/>
-      <c r="G1" s="6" t="s">
+      <c r="F1" s="7"/>
+      <c r="G1" s="7" t="s">
         <v>225</v>
       </c>
-      <c r="H1" s="6"/>
-      <c r="I1" s="6" t="s">
+      <c r="H1" s="7"/>
+      <c r="I1" s="7" t="s">
         <v>546</v>
       </c>
-      <c r="J1" s="6"/>
+      <c r="J1" s="7"/>
     </row>
     <row r="2" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
@@ -2138,10 +2264,10 @@
       <c r="H2" s="3" t="s">
         <v>221</v>
       </c>
-      <c r="I2" s="7" t="s">
+      <c r="I2" s="6" t="s">
         <v>227</v>
       </c>
-      <c r="J2" s="7" t="s">
+      <c r="J2" s="6" t="s">
         <v>221</v>
       </c>
     </row>
@@ -2272,10 +2398,10 @@
       <c r="H6" t="s">
         <v>234</v>
       </c>
-      <c r="I6" s="7" t="s">
+      <c r="I6" s="6" t="s">
         <v>232</v>
       </c>
-      <c r="J6" s="7" t="s">
+      <c r="J6" s="6" t="s">
         <v>30</v>
       </c>
       <c r="Q6" s="2"/>
@@ -2340,10 +2466,10 @@
       <c r="H8" s="3" t="s">
         <v>238</v>
       </c>
-      <c r="I8" s="7" t="s">
+      <c r="I8" s="6" t="s">
         <v>235</v>
       </c>
-      <c r="J8" s="7" t="s">
+      <c r="J8" s="6" t="s">
         <v>236</v>
       </c>
       <c r="Q8" s="2"/>
@@ -2374,10 +2500,10 @@
       <c r="H9" s="3" t="s">
         <v>240</v>
       </c>
-      <c r="I9" s="7" t="s">
+      <c r="I9" s="6" t="s">
         <v>237</v>
       </c>
-      <c r="J9" s="7" t="s">
+      <c r="J9" s="6" t="s">
         <v>238</v>
       </c>
       <c r="Q9" s="2"/>
@@ -2408,10 +2534,10 @@
       <c r="H10" s="3" t="s">
         <v>242</v>
       </c>
-      <c r="I10" s="7" t="s">
+      <c r="I10" s="6" t="s">
         <v>239</v>
       </c>
-      <c r="J10" s="7" t="s">
+      <c r="J10" s="6" t="s">
         <v>240</v>
       </c>
       <c r="Q10" s="2"/>
@@ -2442,10 +2568,10 @@
       <c r="H11" s="3" t="s">
         <v>244</v>
       </c>
-      <c r="I11" s="7" t="s">
+      <c r="I11" s="6" t="s">
         <v>241</v>
       </c>
-      <c r="J11" s="7" t="s">
+      <c r="J11" s="6" t="s">
         <v>242</v>
       </c>
       <c r="Q11" s="2"/>
@@ -2476,10 +2602,10 @@
       <c r="H12" s="3" t="s">
         <v>246</v>
       </c>
-      <c r="I12" s="7" t="s">
+      <c r="I12" s="6" t="s">
         <v>243</v>
       </c>
-      <c r="J12" s="7" t="s">
+      <c r="J12" s="6" t="s">
         <v>244</v>
       </c>
       <c r="Q12" s="2"/>
@@ -2510,10 +2636,10 @@
       <c r="H13" t="s">
         <v>222</v>
       </c>
-      <c r="I13" s="7" t="s">
+      <c r="I13" s="6" t="s">
         <v>245</v>
       </c>
-      <c r="J13" s="7" t="s">
+      <c r="J13" s="6" t="s">
         <v>246</v>
       </c>
       <c r="Q13" s="2"/>
@@ -2816,10 +2942,10 @@
       <c r="H22" s="3" t="s">
         <v>262</v>
       </c>
-      <c r="I22" s="7" t="s">
+      <c r="I22" s="6" t="s">
         <v>259</v>
       </c>
-      <c r="J22" s="7" t="s">
+      <c r="J22" s="6" t="s">
         <v>260</v>
       </c>
       <c r="Q22" s="2"/>
@@ -2884,10 +3010,10 @@
       <c r="H24" t="s">
         <v>265</v>
       </c>
-      <c r="I24" s="7" t="s">
+      <c r="I24" s="6" t="s">
         <v>263</v>
       </c>
-      <c r="J24" s="7" t="s">
+      <c r="J24" s="6" t="s">
         <v>226</v>
       </c>
       <c r="Q24" s="2"/>
@@ -3433,10 +3559,10 @@
       </c>
       <c r="E43" s="1"/>
       <c r="F43" s="1"/>
-      <c r="G43" s="8" t="s">
+      <c r="G43" t="s">
         <v>300</v>
       </c>
-      <c r="H43" s="8" t="s">
+      <c r="H43" t="s">
         <v>301</v>
       </c>
       <c r="I43" s="3" t="s">
@@ -3467,10 +3593,10 @@
       <c r="H44" s="3" t="s">
         <v>303</v>
       </c>
-      <c r="I44" s="8" t="s">
+      <c r="I44" t="s">
         <v>300</v>
       </c>
-      <c r="J44" s="8" t="s">
+      <c r="J44" t="s">
         <v>525</v>
       </c>
     </row>
@@ -3545,10 +3671,10 @@
       </c>
       <c r="E47" s="1"/>
       <c r="F47" s="1"/>
-      <c r="G47" s="8" t="s">
+      <c r="G47" t="s">
         <v>308</v>
       </c>
-      <c r="H47" s="8" t="s">
+      <c r="H47" t="s">
         <v>309</v>
       </c>
       <c r="I47" s="3" t="s">
@@ -3573,16 +3699,16 @@
       </c>
       <c r="E48" s="1"/>
       <c r="F48" s="1"/>
-      <c r="G48" s="8" t="s">
+      <c r="G48" t="s">
         <v>310</v>
       </c>
-      <c r="H48" s="8" t="s">
+      <c r="H48" t="s">
         <v>309</v>
       </c>
-      <c r="I48" s="8" t="s">
+      <c r="I48" t="s">
         <v>308</v>
       </c>
-      <c r="J48" s="8" t="s">
+      <c r="J48" t="s">
         <v>309</v>
       </c>
     </row>
@@ -3601,16 +3727,16 @@
       </c>
       <c r="E49" s="1"/>
       <c r="F49" s="1"/>
-      <c r="G49" s="8" t="s">
+      <c r="G49" t="s">
         <v>311</v>
       </c>
-      <c r="H49" s="8" t="s">
+      <c r="H49" t="s">
         <v>309</v>
       </c>
-      <c r="I49" s="8" t="s">
+      <c r="I49" t="s">
         <v>310</v>
       </c>
-      <c r="J49" s="8" t="s">
+      <c r="J49" t="s">
         <v>309</v>
       </c>
     </row>
@@ -3635,10 +3761,10 @@
       <c r="H50" s="3" t="s">
         <v>313</v>
       </c>
-      <c r="I50" s="8" t="s">
+      <c r="I50" t="s">
         <v>311</v>
       </c>
-      <c r="J50" s="8" t="s">
+      <c r="J50" t="s">
         <v>309</v>
       </c>
     </row>
@@ -3677,10 +3803,10 @@
       <c r="B52" t="s">
         <v>102</v>
       </c>
-      <c r="G52" s="8" t="s">
+      <c r="G52" t="s">
         <v>316</v>
       </c>
-      <c r="H52" s="8" t="s">
+      <c r="H52" t="s">
         <v>317</v>
       </c>
       <c r="I52" s="3" t="s">
@@ -3703,10 +3829,10 @@
       <c r="H53" t="s">
         <v>319</v>
       </c>
-      <c r="I53" s="8" t="s">
+      <c r="I53" t="s">
         <v>316</v>
       </c>
-      <c r="J53" s="8" t="s">
+      <c r="J53" t="s">
         <v>317</v>
       </c>
     </row>
@@ -3823,10 +3949,10 @@
       <c r="H59" s="3" t="s">
         <v>331</v>
       </c>
-      <c r="I59" s="7" t="s">
+      <c r="I59" s="6" t="s">
         <v>326</v>
       </c>
-      <c r="J59" s="7" t="s">
+      <c r="J59" s="6" t="s">
         <v>327</v>
       </c>
     </row>
@@ -4648,7 +4774,240 @@
 </worksheet>
 </file>
 
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7F997DDC-A27B-9E4F-9FC9-66FC153579BE}">
+  <dimension ref="A1:C28"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C7" sqref="C7"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="39.33203125" customWidth="1"/>
+    <col min="3" max="3" width="36" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:3" ht="17" x14ac:dyDescent="0.2">
+      <c r="A1" s="8" t="s">
+        <v>547</v>
+      </c>
+      <c r="C1" s="8" t="s">
+        <v>556</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" ht="17" x14ac:dyDescent="0.2">
+      <c r="A2" s="9" t="s">
+        <v>548</v>
+      </c>
+      <c r="C2" s="9" t="s">
+        <v>554</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" ht="17" x14ac:dyDescent="0.2">
+      <c r="A3" s="9" t="s">
+        <v>549</v>
+      </c>
+      <c r="C3" s="9" t="s">
+        <v>555</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" ht="17" x14ac:dyDescent="0.2">
+      <c r="A4" s="9" t="s">
+        <v>550</v>
+      </c>
+      <c r="C4" s="9" t="s">
+        <v>550</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" ht="17" x14ac:dyDescent="0.2">
+      <c r="A5" s="9" t="s">
+        <v>551</v>
+      </c>
+      <c r="C5" s="9" t="s">
+        <v>551</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" ht="17" x14ac:dyDescent="0.2">
+      <c r="A6" s="9" t="s">
+        <v>552</v>
+      </c>
+      <c r="C6" s="9" t="s">
+        <v>552</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3" ht="17" x14ac:dyDescent="0.2">
+      <c r="A7" s="10" t="s">
+        <v>553</v>
+      </c>
+      <c r="C7" s="10" t="s">
+        <v>553</v>
+      </c>
+    </row>
+    <row r="9" spans="1:3" ht="34" x14ac:dyDescent="0.2">
+      <c r="A9" s="12" t="s">
+        <v>557</v>
+      </c>
+      <c r="C9" s="11"/>
+    </row>
+    <row r="10" spans="1:3" ht="34" x14ac:dyDescent="0.2">
+      <c r="A10" s="10" t="s">
+        <v>558</v>
+      </c>
+      <c r="C10" s="10" t="s">
+        <v>558</v>
+      </c>
+    </row>
+    <row r="11" spans="1:3" ht="34" x14ac:dyDescent="0.2">
+      <c r="A11" s="10" t="s">
+        <v>559</v>
+      </c>
+      <c r="C11" s="10" t="s">
+        <v>559</v>
+      </c>
+    </row>
+    <row r="12" spans="1:3" ht="34" x14ac:dyDescent="0.2">
+      <c r="A12" s="10" t="s">
+        <v>560</v>
+      </c>
+      <c r="C12" s="10" t="s">
+        <v>560</v>
+      </c>
+    </row>
+    <row r="13" spans="1:3" ht="34" x14ac:dyDescent="0.2">
+      <c r="A13" s="10" t="s">
+        <v>561</v>
+      </c>
+      <c r="C13" s="10" t="s">
+        <v>561</v>
+      </c>
+    </row>
+    <row r="14" spans="1:3" ht="17" x14ac:dyDescent="0.2">
+      <c r="A14" s="10" t="s">
+        <v>562</v>
+      </c>
+      <c r="C14" s="10" t="s">
+        <v>562</v>
+      </c>
+    </row>
+    <row r="15" spans="1:3" ht="17" x14ac:dyDescent="0.2">
+      <c r="A15" s="10" t="s">
+        <v>563</v>
+      </c>
+      <c r="C15" s="10" t="s">
+        <v>563</v>
+      </c>
+    </row>
+    <row r="16" spans="1:3" ht="17" x14ac:dyDescent="0.2">
+      <c r="A16" s="10" t="s">
+        <v>564</v>
+      </c>
+      <c r="C16" s="10" t="s">
+        <v>564</v>
+      </c>
+    </row>
+    <row r="17" spans="1:3" ht="17" x14ac:dyDescent="0.2">
+      <c r="A17" s="10" t="s">
+        <v>565</v>
+      </c>
+      <c r="C17" s="10" t="s">
+        <v>565</v>
+      </c>
+    </row>
+    <row r="18" spans="1:3" ht="34" x14ac:dyDescent="0.2">
+      <c r="A18" s="10" t="s">
+        <v>566</v>
+      </c>
+      <c r="C18" s="12" t="s">
+        <v>567</v>
+      </c>
+    </row>
+    <row r="20" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A20" s="11" t="s">
+        <v>568</v>
+      </c>
+      <c r="C20" s="11" t="s">
+        <v>568</v>
+      </c>
+    </row>
+    <row r="21" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A21" s="11" t="s">
+        <v>569</v>
+      </c>
+      <c r="C21" s="11" t="s">
+        <v>569</v>
+      </c>
+    </row>
+    <row r="22" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A22" s="11" t="s">
+        <v>570</v>
+      </c>
+      <c r="C22" s="11" t="s">
+        <v>570</v>
+      </c>
+    </row>
+    <row r="23" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A23" s="11" t="s">
+        <v>571</v>
+      </c>
+      <c r="C23" s="11" t="s">
+        <v>571</v>
+      </c>
+    </row>
+    <row r="24" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A24" s="11" t="s">
+        <v>572</v>
+      </c>
+      <c r="C24" s="11" t="s">
+        <v>572</v>
+      </c>
+    </row>
+    <row r="25" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A25" s="11" t="s">
+        <v>573</v>
+      </c>
+      <c r="C25" s="11" t="s">
+        <v>573</v>
+      </c>
+    </row>
+    <row r="26" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A26" s="11" t="s">
+        <v>574</v>
+      </c>
+      <c r="C26" s="11" t="s">
+        <v>574</v>
+      </c>
+    </row>
+    <row r="27" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A27" s="11" t="s">
+        <v>575</v>
+      </c>
+      <c r="C27" s="11" t="s">
+        <v>575</v>
+      </c>
+    </row>
+    <row r="28" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A28" s="13" t="s">
+        <v>576</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <TaxCatchAll xmlns="d391a701-1e72-4a9c-8e27-32ae852ac85b" xsi:nil="true"/>
+    <lcf76f155ced4ddcb4097134ff3c332f xmlns="748de206-7911-403a-93a2-ff3feb5ad88e">
+      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    </lcf76f155ced4ddcb4097134ff3c332f>
+  </documentManagement>
+</p:properties>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x0101009FE99232C2A610489C05CA2A95C6B0DC" ma:contentTypeVersion="16" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="99e3d855f4612a477f80c26c84225e60">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="748de206-7911-403a-93a2-ff3feb5ad88e" xmlns:ns3="d391a701-1e72-4a9c-8e27-32ae852ac85b" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="9d24ec2972380c9becf470258562e41c" ns2:_="" ns3:_="">
     <xsd:import namespace="748de206-7911-403a-93a2-ff3feb5ad88e"/>
@@ -4879,17 +5238,6 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <TaxCatchAll xmlns="d391a701-1e72-4a9c-8e27-32ae852ac85b" xsi:nil="true"/>
-    <lcf76f155ced4ddcb4097134ff3c332f xmlns="748de206-7911-403a-93a2-ff3feb5ad88e">
-      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    </lcf76f155ced4ddcb4097134ff3c332f>
-  </documentManagement>
-</p:properties>
-</file>
-
 <file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <?mso-contentType ?>
 <FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
@@ -4900,6 +5248,23 @@
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{8A0F7ED7-B064-47CF-BC44-4A045BE18651}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="748de206-7911-403a-93a2-ff3feb5ad88e"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="d391a701-1e72-4a9c-8e27-32ae852ac85b"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{425960D1-4FA0-44B7-8D5C-E9238875A675}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -4918,23 +5283,6 @@
 </ds:datastoreItem>
 </file>
 
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{8A0F7ED7-B064-47CF-BC44-4A045BE18651}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="d391a701-1e72-4a9c-8e27-32ae852ac85b"/>
-    <ds:schemaRef ds:uri="748de206-7911-403a-93a2-ff3feb5ad88e"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{FBF3EE50-7D40-453B-9B2A-4D1C4E8CD157}">
   <ds:schemaRefs>

</xml_diff>

<commit_message>
updated wealth quantile graphs + design
</commit_message>
<xml_diff>
--- a/AssetSurveyItems_Match.xlsx
+++ b/AssetSurveyItems_Match.xlsx
@@ -1,20 +1,19 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11113"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11011"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://mcgill.sharepoint.com/sites/PROSPERED_Group/Shared Documents/General/CIHR RSBY India/data/Linking code and CSVs/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="97" documentId="8_{F77C4B80-A99E-7F40-A288-258E5FEBB2B2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{24427BF8-F743-1A4B-B820-01594330A9B0}"/>
+  <xr:revisionPtr revIDLastSave="29" documentId="8_{F77C4B80-A99E-7F40-A288-258E5FEBB2B2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{7D926B75-DE62-D845-B523-0A43FED8E1B3}"/>
   <bookViews>
-    <workbookView xWindow="13800" yWindow="500" windowWidth="20480" windowHeight="16520" activeTab="1" xr2:uid="{87D403AE-B090-804E-AAD5-1AA8BD4EAB0C}"/>
+    <workbookView xWindow="2900" yWindow="500" windowWidth="20480" windowHeight="16520" xr2:uid="{87D403AE-B090-804E-AAD5-1AA8BD4EAB0C}"/>
   </bookViews>
   <sheets>
-    <sheet name="Across Survyes" sheetId="1" r:id="rId1"/>
-    <sheet name="Correct order for AI" sheetId="2" r:id="rId2"/>
+    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
   <calcPr calcId="181029"/>
   <extLst>
@@ -37,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="775" uniqueCount="577">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="725" uniqueCount="547">
   <si>
     <t>DLHS3</t>
   </si>
@@ -1678,96 +1677,6 @@
   </si>
   <si>
     <t>NFHS5</t>
-  </si>
-  <si>
-    <t xml:space="preserve">  1   piped-water-into-dwelling-yardplot</t>
-  </si>
-  <si>
-    <t xml:space="preserve">           2   public-tap-stand-pipe</t>
-  </si>
-  <si>
-    <t xml:space="preserve">           3  tubewell-or-borehole</t>
-  </si>
-  <si>
-    <t xml:space="preserve">           4   protected-dugwell</t>
-  </si>
-  <si>
-    <t xml:space="preserve">           5   unprotected-dug-well</t>
-  </si>
-  <si>
-    <t>6 tanker/truck/cart</t>
-  </si>
-  <si>
-    <t>7other source</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> 2   public-tap-stand-pipe</t>
-  </si>
-  <si>
-    <t>3  tubewell-or-borehole</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> 1   piped-water-into-dwelling-yardplot</t>
-  </si>
-  <si>
-    <t>0 OPEN DEFECATION/NO FACILITY/OPEN SPACE OR FIELD</t>
-  </si>
-  <si>
-    <t xml:space="preserve">1 pour/flush latrine: connected to piped sewer system </t>
-  </si>
-  <si>
-    <t xml:space="preserve">2 pour/flush latrine: connected to septic tank </t>
-  </si>
-  <si>
-    <t xml:space="preserve">3 pour/flush latrine: connected to pit latrine </t>
-  </si>
-  <si>
-    <t xml:space="preserve">4 pour/flush latrine: connected to something else </t>
-  </si>
-  <si>
-    <t xml:space="preserve">5 pit latrine: ventilated improved pit </t>
-  </si>
-  <si>
-    <t xml:space="preserve">6 pit latrine: with slab </t>
-  </si>
-  <si>
-    <t xml:space="preserve">7 pit latrine: open or without slab </t>
-  </si>
-  <si>
-    <t>8 service latrine /dry toilet</t>
-  </si>
-  <si>
-    <t>9 OTHER</t>
-  </si>
-  <si>
-    <t>9 OPEN DEFECATION/NO FACILITY/OPEN SPACE OR FIELD</t>
-  </si>
-  <si>
-    <t>1 Electricity</t>
-  </si>
-  <si>
-    <t>2 LPG/ Natural Gas</t>
-  </si>
-  <si>
-    <t>3 Biogas</t>
-  </si>
-  <si>
-    <t>4 Kerosene</t>
-  </si>
-  <si>
-    <t>5 Coal / Ignite / Charcoal</t>
-  </si>
-  <si>
-    <t>6 Wood</t>
-  </si>
-  <si>
-    <t>7 Straw / Shrubs / Grass / Agricultural Crop Waste</t>
-  </si>
-  <si>
-    <t>8 Dung Cakes</t>
-  </si>
-  <si>
-    <t>96 Other</t>
   </si>
 </sst>
 </file>
@@ -1824,7 +1733,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="3">
+  <borders count="1">
     <border>
       <left/>
       <right/>
@@ -1832,53 +1741,22 @@
       <bottom/>
       <diagonal/>
     </border>
-    <border>
-      <left/>
-      <right/>
-      <top style="thin">
-        <color indexed="64"/>
-      </top>
-      <bottom/>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="thin">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="14">
+  <cellXfs count="9">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1894,10 +1772,6 @@
     </ext>
   </extLst>
 </styleSheet>
-</file>
-
-<file path=xl/persons/person.xml><?xml version="1.0" encoding="utf-8"?>
-<personList xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -2199,7 +2073,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{55E3B49A-77A0-AD4A-81B0-B8BFD615B07C}">
   <dimension ref="A1:S132"/>
   <sheetViews>
-    <sheetView topLeftCell="I1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="I1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A38" activePane="bottomLeft" state="frozen"/>
       <selection activeCell="D1" sqref="D1"/>
       <selection pane="bottomLeft" activeCell="I59" sqref="I59:J59"/>
@@ -2218,26 +2092,26 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:18" x14ac:dyDescent="0.2">
-      <c r="A1" s="7" t="s">
+      <c r="A1" s="6" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="7"/>
-      <c r="C1" s="7" t="s">
+      <c r="B1" s="6"/>
+      <c r="C1" s="6" t="s">
         <v>121</v>
       </c>
-      <c r="D1" s="7"/>
-      <c r="E1" s="7" t="s">
+      <c r="D1" s="6"/>
+      <c r="E1" s="6" t="s">
         <v>470</v>
       </c>
-      <c r="F1" s="7"/>
-      <c r="G1" s="7" t="s">
+      <c r="F1" s="6"/>
+      <c r="G1" s="6" t="s">
         <v>225</v>
       </c>
-      <c r="H1" s="7"/>
-      <c r="I1" s="7" t="s">
+      <c r="H1" s="6"/>
+      <c r="I1" s="6" t="s">
         <v>546</v>
       </c>
-      <c r="J1" s="7"/>
+      <c r="J1" s="6"/>
     </row>
     <row r="2" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
@@ -2264,10 +2138,10 @@
       <c r="H2" s="3" t="s">
         <v>221</v>
       </c>
-      <c r="I2" s="6" t="s">
+      <c r="I2" s="7" t="s">
         <v>227</v>
       </c>
-      <c r="J2" s="6" t="s">
+      <c r="J2" s="7" t="s">
         <v>221</v>
       </c>
     </row>
@@ -2398,10 +2272,10 @@
       <c r="H6" t="s">
         <v>234</v>
       </c>
-      <c r="I6" s="6" t="s">
+      <c r="I6" s="7" t="s">
         <v>232</v>
       </c>
-      <c r="J6" s="6" t="s">
+      <c r="J6" s="7" t="s">
         <v>30</v>
       </c>
       <c r="Q6" s="2"/>
@@ -2466,10 +2340,10 @@
       <c r="H8" s="3" t="s">
         <v>238</v>
       </c>
-      <c r="I8" s="6" t="s">
+      <c r="I8" s="7" t="s">
         <v>235</v>
       </c>
-      <c r="J8" s="6" t="s">
+      <c r="J8" s="7" t="s">
         <v>236</v>
       </c>
       <c r="Q8" s="2"/>
@@ -2500,10 +2374,10 @@
       <c r="H9" s="3" t="s">
         <v>240</v>
       </c>
-      <c r="I9" s="6" t="s">
+      <c r="I9" s="7" t="s">
         <v>237</v>
       </c>
-      <c r="J9" s="6" t="s">
+      <c r="J9" s="7" t="s">
         <v>238</v>
       </c>
       <c r="Q9" s="2"/>
@@ -2534,10 +2408,10 @@
       <c r="H10" s="3" t="s">
         <v>242</v>
       </c>
-      <c r="I10" s="6" t="s">
+      <c r="I10" s="7" t="s">
         <v>239</v>
       </c>
-      <c r="J10" s="6" t="s">
+      <c r="J10" s="7" t="s">
         <v>240</v>
       </c>
       <c r="Q10" s="2"/>
@@ -2568,10 +2442,10 @@
       <c r="H11" s="3" t="s">
         <v>244</v>
       </c>
-      <c r="I11" s="6" t="s">
+      <c r="I11" s="7" t="s">
         <v>241</v>
       </c>
-      <c r="J11" s="6" t="s">
+      <c r="J11" s="7" t="s">
         <v>242</v>
       </c>
       <c r="Q11" s="2"/>
@@ -2602,10 +2476,10 @@
       <c r="H12" s="3" t="s">
         <v>246</v>
       </c>
-      <c r="I12" s="6" t="s">
+      <c r="I12" s="7" t="s">
         <v>243</v>
       </c>
-      <c r="J12" s="6" t="s">
+      <c r="J12" s="7" t="s">
         <v>244</v>
       </c>
       <c r="Q12" s="2"/>
@@ -2636,10 +2510,10 @@
       <c r="H13" t="s">
         <v>222</v>
       </c>
-      <c r="I13" s="6" t="s">
+      <c r="I13" s="7" t="s">
         <v>245</v>
       </c>
-      <c r="J13" s="6" t="s">
+      <c r="J13" s="7" t="s">
         <v>246</v>
       </c>
       <c r="Q13" s="2"/>
@@ -2942,10 +2816,10 @@
       <c r="H22" s="3" t="s">
         <v>262</v>
       </c>
-      <c r="I22" s="6" t="s">
+      <c r="I22" s="7" t="s">
         <v>259</v>
       </c>
-      <c r="J22" s="6" t="s">
+      <c r="J22" s="7" t="s">
         <v>260</v>
       </c>
       <c r="Q22" s="2"/>
@@ -3010,10 +2884,10 @@
       <c r="H24" t="s">
         <v>265</v>
       </c>
-      <c r="I24" s="6" t="s">
+      <c r="I24" s="7" t="s">
         <v>263</v>
       </c>
-      <c r="J24" s="6" t="s">
+      <c r="J24" s="7" t="s">
         <v>226</v>
       </c>
       <c r="Q24" s="2"/>
@@ -3559,10 +3433,10 @@
       </c>
       <c r="E43" s="1"/>
       <c r="F43" s="1"/>
-      <c r="G43" t="s">
+      <c r="G43" s="8" t="s">
         <v>300</v>
       </c>
-      <c r="H43" t="s">
+      <c r="H43" s="8" t="s">
         <v>301</v>
       </c>
       <c r="I43" s="3" t="s">
@@ -3593,10 +3467,10 @@
       <c r="H44" s="3" t="s">
         <v>303</v>
       </c>
-      <c r="I44" t="s">
+      <c r="I44" s="8" t="s">
         <v>300</v>
       </c>
-      <c r="J44" t="s">
+      <c r="J44" s="8" t="s">
         <v>525</v>
       </c>
     </row>
@@ -3671,10 +3545,10 @@
       </c>
       <c r="E47" s="1"/>
       <c r="F47" s="1"/>
-      <c r="G47" t="s">
+      <c r="G47" s="8" t="s">
         <v>308</v>
       </c>
-      <c r="H47" t="s">
+      <c r="H47" s="8" t="s">
         <v>309</v>
       </c>
       <c r="I47" s="3" t="s">
@@ -3699,16 +3573,16 @@
       </c>
       <c r="E48" s="1"/>
       <c r="F48" s="1"/>
-      <c r="G48" t="s">
+      <c r="G48" s="8" t="s">
         <v>310</v>
       </c>
-      <c r="H48" t="s">
+      <c r="H48" s="8" t="s">
         <v>309</v>
       </c>
-      <c r="I48" t="s">
+      <c r="I48" s="8" t="s">
         <v>308</v>
       </c>
-      <c r="J48" t="s">
+      <c r="J48" s="8" t="s">
         <v>309</v>
       </c>
     </row>
@@ -3727,16 +3601,16 @@
       </c>
       <c r="E49" s="1"/>
       <c r="F49" s="1"/>
-      <c r="G49" t="s">
+      <c r="G49" s="8" t="s">
         <v>311</v>
       </c>
-      <c r="H49" t="s">
+      <c r="H49" s="8" t="s">
         <v>309</v>
       </c>
-      <c r="I49" t="s">
+      <c r="I49" s="8" t="s">
         <v>310</v>
       </c>
-      <c r="J49" t="s">
+      <c r="J49" s="8" t="s">
         <v>309</v>
       </c>
     </row>
@@ -3761,10 +3635,10 @@
       <c r="H50" s="3" t="s">
         <v>313</v>
       </c>
-      <c r="I50" t="s">
+      <c r="I50" s="8" t="s">
         <v>311</v>
       </c>
-      <c r="J50" t="s">
+      <c r="J50" s="8" t="s">
         <v>309</v>
       </c>
     </row>
@@ -3803,10 +3677,10 @@
       <c r="B52" t="s">
         <v>102</v>
       </c>
-      <c r="G52" t="s">
+      <c r="G52" s="8" t="s">
         <v>316</v>
       </c>
-      <c r="H52" t="s">
+      <c r="H52" s="8" t="s">
         <v>317</v>
       </c>
       <c r="I52" s="3" t="s">
@@ -3829,10 +3703,10 @@
       <c r="H53" t="s">
         <v>319</v>
       </c>
-      <c r="I53" t="s">
+      <c r="I53" s="8" t="s">
         <v>316</v>
       </c>
-      <c r="J53" t="s">
+      <c r="J53" s="8" t="s">
         <v>317</v>
       </c>
     </row>
@@ -3949,10 +3823,10 @@
       <c r="H59" s="3" t="s">
         <v>331</v>
       </c>
-      <c r="I59" s="6" t="s">
+      <c r="I59" s="7" t="s">
         <v>326</v>
       </c>
-      <c r="J59" s="6" t="s">
+      <c r="J59" s="7" t="s">
         <v>327</v>
       </c>
     </row>
@@ -4774,240 +4648,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7F997DDC-A27B-9E4F-9FC9-66FC153579BE}">
-  <dimension ref="A1:C28"/>
-  <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C7" sqref="C7"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
-  <cols>
-    <col min="1" max="1" width="39.33203125" customWidth="1"/>
-    <col min="3" max="3" width="36" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:3" ht="17" x14ac:dyDescent="0.2">
-      <c r="A1" s="8" t="s">
-        <v>547</v>
-      </c>
-      <c r="C1" s="8" t="s">
-        <v>556</v>
-      </c>
-    </row>
-    <row r="2" spans="1:3" ht="17" x14ac:dyDescent="0.2">
-      <c r="A2" s="9" t="s">
-        <v>548</v>
-      </c>
-      <c r="C2" s="9" t="s">
-        <v>554</v>
-      </c>
-    </row>
-    <row r="3" spans="1:3" ht="17" x14ac:dyDescent="0.2">
-      <c r="A3" s="9" t="s">
-        <v>549</v>
-      </c>
-      <c r="C3" s="9" t="s">
-        <v>555</v>
-      </c>
-    </row>
-    <row r="4" spans="1:3" ht="17" x14ac:dyDescent="0.2">
-      <c r="A4" s="9" t="s">
-        <v>550</v>
-      </c>
-      <c r="C4" s="9" t="s">
-        <v>550</v>
-      </c>
-    </row>
-    <row r="5" spans="1:3" ht="17" x14ac:dyDescent="0.2">
-      <c r="A5" s="9" t="s">
-        <v>551</v>
-      </c>
-      <c r="C5" s="9" t="s">
-        <v>551</v>
-      </c>
-    </row>
-    <row r="6" spans="1:3" ht="17" x14ac:dyDescent="0.2">
-      <c r="A6" s="9" t="s">
-        <v>552</v>
-      </c>
-      <c r="C6" s="9" t="s">
-        <v>552</v>
-      </c>
-    </row>
-    <row r="7" spans="1:3" ht="17" x14ac:dyDescent="0.2">
-      <c r="A7" s="10" t="s">
-        <v>553</v>
-      </c>
-      <c r="C7" s="10" t="s">
-        <v>553</v>
-      </c>
-    </row>
-    <row r="9" spans="1:3" ht="34" x14ac:dyDescent="0.2">
-      <c r="A9" s="12" t="s">
-        <v>557</v>
-      </c>
-      <c r="C9" s="11"/>
-    </row>
-    <row r="10" spans="1:3" ht="34" x14ac:dyDescent="0.2">
-      <c r="A10" s="10" t="s">
-        <v>558</v>
-      </c>
-      <c r="C10" s="10" t="s">
-        <v>558</v>
-      </c>
-    </row>
-    <row r="11" spans="1:3" ht="34" x14ac:dyDescent="0.2">
-      <c r="A11" s="10" t="s">
-        <v>559</v>
-      </c>
-      <c r="C11" s="10" t="s">
-        <v>559</v>
-      </c>
-    </row>
-    <row r="12" spans="1:3" ht="34" x14ac:dyDescent="0.2">
-      <c r="A12" s="10" t="s">
-        <v>560</v>
-      </c>
-      <c r="C12" s="10" t="s">
-        <v>560</v>
-      </c>
-    </row>
-    <row r="13" spans="1:3" ht="34" x14ac:dyDescent="0.2">
-      <c r="A13" s="10" t="s">
-        <v>561</v>
-      </c>
-      <c r="C13" s="10" t="s">
-        <v>561</v>
-      </c>
-    </row>
-    <row r="14" spans="1:3" ht="17" x14ac:dyDescent="0.2">
-      <c r="A14" s="10" t="s">
-        <v>562</v>
-      </c>
-      <c r="C14" s="10" t="s">
-        <v>562</v>
-      </c>
-    </row>
-    <row r="15" spans="1:3" ht="17" x14ac:dyDescent="0.2">
-      <c r="A15" s="10" t="s">
-        <v>563</v>
-      </c>
-      <c r="C15" s="10" t="s">
-        <v>563</v>
-      </c>
-    </row>
-    <row r="16" spans="1:3" ht="17" x14ac:dyDescent="0.2">
-      <c r="A16" s="10" t="s">
-        <v>564</v>
-      </c>
-      <c r="C16" s="10" t="s">
-        <v>564</v>
-      </c>
-    </row>
-    <row r="17" spans="1:3" ht="17" x14ac:dyDescent="0.2">
-      <c r="A17" s="10" t="s">
-        <v>565</v>
-      </c>
-      <c r="C17" s="10" t="s">
-        <v>565</v>
-      </c>
-    </row>
-    <row r="18" spans="1:3" ht="34" x14ac:dyDescent="0.2">
-      <c r="A18" s="10" t="s">
-        <v>566</v>
-      </c>
-      <c r="C18" s="12" t="s">
-        <v>567</v>
-      </c>
-    </row>
-    <row r="20" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A20" s="11" t="s">
-        <v>568</v>
-      </c>
-      <c r="C20" s="11" t="s">
-        <v>568</v>
-      </c>
-    </row>
-    <row r="21" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A21" s="11" t="s">
-        <v>569</v>
-      </c>
-      <c r="C21" s="11" t="s">
-        <v>569</v>
-      </c>
-    </row>
-    <row r="22" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A22" s="11" t="s">
-        <v>570</v>
-      </c>
-      <c r="C22" s="11" t="s">
-        <v>570</v>
-      </c>
-    </row>
-    <row r="23" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A23" s="11" t="s">
-        <v>571</v>
-      </c>
-      <c r="C23" s="11" t="s">
-        <v>571</v>
-      </c>
-    </row>
-    <row r="24" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A24" s="11" t="s">
-        <v>572</v>
-      </c>
-      <c r="C24" s="11" t="s">
-        <v>572</v>
-      </c>
-    </row>
-    <row r="25" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A25" s="11" t="s">
-        <v>573</v>
-      </c>
-      <c r="C25" s="11" t="s">
-        <v>573</v>
-      </c>
-    </row>
-    <row r="26" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A26" s="11" t="s">
-        <v>574</v>
-      </c>
-      <c r="C26" s="11" t="s">
-        <v>574</v>
-      </c>
-    </row>
-    <row r="27" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A27" s="11" t="s">
-        <v>575</v>
-      </c>
-      <c r="C27" s="11" t="s">
-        <v>575</v>
-      </c>
-    </row>
-    <row r="28" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A28" s="13" t="s">
-        <v>576</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <TaxCatchAll xmlns="d391a701-1e72-4a9c-8e27-32ae852ac85b" xsi:nil="true"/>
-    <lcf76f155ced4ddcb4097134ff3c332f xmlns="748de206-7911-403a-93a2-ff3feb5ad88e">
-      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    </lcf76f155ced4ddcb4097134ff3c332f>
-  </documentManagement>
-</p:properties>
-</file>
-
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x0101009FE99232C2A610489C05CA2A95C6B0DC" ma:contentTypeVersion="16" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="99e3d855f4612a477f80c26c84225e60">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="748de206-7911-403a-93a2-ff3feb5ad88e" xmlns:ns3="d391a701-1e72-4a9c-8e27-32ae852ac85b" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="9d24ec2972380c9becf470258562e41c" ns2:_="" ns3:_="">
     <xsd:import namespace="748de206-7911-403a-93a2-ff3feb5ad88e"/>
@@ -5238,6 +4879,17 @@
 </ct:contentTypeSchema>
 </file>
 
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <TaxCatchAll xmlns="d391a701-1e72-4a9c-8e27-32ae852ac85b" xsi:nil="true"/>
+    <lcf76f155ced4ddcb4097134ff3c332f xmlns="748de206-7911-403a-93a2-ff3feb5ad88e">
+      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    </lcf76f155ced4ddcb4097134ff3c332f>
+  </documentManagement>
+</p:properties>
+</file>
+
 <file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <?mso-contentType ?>
 <FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
@@ -5248,23 +4900,6 @@
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{8A0F7ED7-B064-47CF-BC44-4A045BE18651}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <ds:schemaRef ds:uri="748de206-7911-403a-93a2-ff3feb5ad88e"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-    <ds:schemaRef ds:uri="d391a701-1e72-4a9c-8e27-32ae852ac85b"/>
-    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{425960D1-4FA0-44B7-8D5C-E9238875A675}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -5283,6 +4918,23 @@
 </ds:datastoreItem>
 </file>
 
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{8A0F7ED7-B064-47CF-BC44-4A045BE18651}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="d391a701-1e72-4a9c-8e27-32ae852ac85b"/>
+    <ds:schemaRef ds:uri="748de206-7911-403a-93a2-ff3feb5ad88e"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{FBF3EE50-7D40-453B-9B2A-4D1C4E8CD157}">
   <ds:schemaRefs>

</xml_diff>

<commit_message>
wealth index and weight denormalization
</commit_message>
<xml_diff>
--- a/AssetSurveyItems_Match.xlsx
+++ b/AssetSurveyItems_Match.xlsx
@@ -1,19 +1,20 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11011"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11113"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://mcgill.sharepoint.com/sites/PROSPERED_Group/Shared Documents/General/CIHR RSBY India/data/Linking code and CSVs/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="29" documentId="8_{F77C4B80-A99E-7F40-A288-258E5FEBB2B2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{7D926B75-DE62-D845-B523-0A43FED8E1B3}"/>
+  <xr:revisionPtr revIDLastSave="97" documentId="8_{F77C4B80-A99E-7F40-A288-258E5FEBB2B2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{24427BF8-F743-1A4B-B820-01594330A9B0}"/>
   <bookViews>
-    <workbookView xWindow="2900" yWindow="500" windowWidth="20480" windowHeight="16520" xr2:uid="{87D403AE-B090-804E-AAD5-1AA8BD4EAB0C}"/>
+    <workbookView xWindow="13800" yWindow="500" windowWidth="20480" windowHeight="16520" activeTab="1" xr2:uid="{87D403AE-B090-804E-AAD5-1AA8BD4EAB0C}"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="Across Survyes" sheetId="1" r:id="rId1"/>
+    <sheet name="Correct order for AI" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="181029"/>
   <extLst>
@@ -36,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="725" uniqueCount="547">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="775" uniqueCount="577">
   <si>
     <t>DLHS3</t>
   </si>
@@ -1677,6 +1678,96 @@
   </si>
   <si>
     <t>NFHS5</t>
+  </si>
+  <si>
+    <t xml:space="preserve">  1   piped-water-into-dwelling-yardplot</t>
+  </si>
+  <si>
+    <t xml:space="preserve">           2   public-tap-stand-pipe</t>
+  </si>
+  <si>
+    <t xml:space="preserve">           3  tubewell-or-borehole</t>
+  </si>
+  <si>
+    <t xml:space="preserve">           4   protected-dugwell</t>
+  </si>
+  <si>
+    <t xml:space="preserve">           5   unprotected-dug-well</t>
+  </si>
+  <si>
+    <t>6 tanker/truck/cart</t>
+  </si>
+  <si>
+    <t>7other source</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 2   public-tap-stand-pipe</t>
+  </si>
+  <si>
+    <t>3  tubewell-or-borehole</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 1   piped-water-into-dwelling-yardplot</t>
+  </si>
+  <si>
+    <t>0 OPEN DEFECATION/NO FACILITY/OPEN SPACE OR FIELD</t>
+  </si>
+  <si>
+    <t xml:space="preserve">1 pour/flush latrine: connected to piped sewer system </t>
+  </si>
+  <si>
+    <t xml:space="preserve">2 pour/flush latrine: connected to septic tank </t>
+  </si>
+  <si>
+    <t xml:space="preserve">3 pour/flush latrine: connected to pit latrine </t>
+  </si>
+  <si>
+    <t xml:space="preserve">4 pour/flush latrine: connected to something else </t>
+  </si>
+  <si>
+    <t xml:space="preserve">5 pit latrine: ventilated improved pit </t>
+  </si>
+  <si>
+    <t xml:space="preserve">6 pit latrine: with slab </t>
+  </si>
+  <si>
+    <t xml:space="preserve">7 pit latrine: open or without slab </t>
+  </si>
+  <si>
+    <t>8 service latrine /dry toilet</t>
+  </si>
+  <si>
+    <t>9 OTHER</t>
+  </si>
+  <si>
+    <t>9 OPEN DEFECATION/NO FACILITY/OPEN SPACE OR FIELD</t>
+  </si>
+  <si>
+    <t>1 Electricity</t>
+  </si>
+  <si>
+    <t>2 LPG/ Natural Gas</t>
+  </si>
+  <si>
+    <t>3 Biogas</t>
+  </si>
+  <si>
+    <t>4 Kerosene</t>
+  </si>
+  <si>
+    <t>5 Coal / Ignite / Charcoal</t>
+  </si>
+  <si>
+    <t>6 Wood</t>
+  </si>
+  <si>
+    <t>7 Straw / Shrubs / Grass / Agricultural Crop Waste</t>
+  </si>
+  <si>
+    <t>8 Dung Cakes</t>
+  </si>
+  <si>
+    <t>96 Other</t>
   </si>
 </sst>
 </file>
@@ -1733,7 +1824,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="1">
+  <borders count="3">
     <border>
       <left/>
       <right/>
@@ -1741,22 +1832,53 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="9">
+  <cellXfs count="14">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1772,6 +1894,10 @@
     </ext>
   </extLst>
 </styleSheet>
+</file>
+
+<file path=xl/persons/person.xml><?xml version="1.0" encoding="utf-8"?>
+<personList xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -2073,7 +2199,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{55E3B49A-77A0-AD4A-81B0-B8BFD615B07C}">
   <dimension ref="A1:S132"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="I1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+    <sheetView topLeftCell="I1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A38" activePane="bottomLeft" state="frozen"/>
       <selection activeCell="D1" sqref="D1"/>
       <selection pane="bottomLeft" activeCell="I59" sqref="I59:J59"/>
@@ -2092,26 +2218,26 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:18" x14ac:dyDescent="0.2">
-      <c r="A1" s="6" t="s">
+      <c r="A1" s="7" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="6"/>
-      <c r="C1" s="6" t="s">
+      <c r="B1" s="7"/>
+      <c r="C1" s="7" t="s">
         <v>121</v>
       </c>
-      <c r="D1" s="6"/>
-      <c r="E1" s="6" t="s">
+      <c r="D1" s="7"/>
+      <c r="E1" s="7" t="s">
         <v>470</v>
       </c>
-      <c r="F1" s="6"/>
-      <c r="G1" s="6" t="s">
+      <c r="F1" s="7"/>
+      <c r="G1" s="7" t="s">
         <v>225</v>
       </c>
-      <c r="H1" s="6"/>
-      <c r="I1" s="6" t="s">
+      <c r="H1" s="7"/>
+      <c r="I1" s="7" t="s">
         <v>546</v>
       </c>
-      <c r="J1" s="6"/>
+      <c r="J1" s="7"/>
     </row>
     <row r="2" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
@@ -2138,10 +2264,10 @@
       <c r="H2" s="3" t="s">
         <v>221</v>
       </c>
-      <c r="I2" s="7" t="s">
+      <c r="I2" s="6" t="s">
         <v>227</v>
       </c>
-      <c r="J2" s="7" t="s">
+      <c r="J2" s="6" t="s">
         <v>221</v>
       </c>
     </row>
@@ -2272,10 +2398,10 @@
       <c r="H6" t="s">
         <v>234</v>
       </c>
-      <c r="I6" s="7" t="s">
+      <c r="I6" s="6" t="s">
         <v>232</v>
       </c>
-      <c r="J6" s="7" t="s">
+      <c r="J6" s="6" t="s">
         <v>30</v>
       </c>
       <c r="Q6" s="2"/>
@@ -2340,10 +2466,10 @@
       <c r="H8" s="3" t="s">
         <v>238</v>
       </c>
-      <c r="I8" s="7" t="s">
+      <c r="I8" s="6" t="s">
         <v>235</v>
       </c>
-      <c r="J8" s="7" t="s">
+      <c r="J8" s="6" t="s">
         <v>236</v>
       </c>
       <c r="Q8" s="2"/>
@@ -2374,10 +2500,10 @@
       <c r="H9" s="3" t="s">
         <v>240</v>
       </c>
-      <c r="I9" s="7" t="s">
+      <c r="I9" s="6" t="s">
         <v>237</v>
       </c>
-      <c r="J9" s="7" t="s">
+      <c r="J9" s="6" t="s">
         <v>238</v>
       </c>
       <c r="Q9" s="2"/>
@@ -2408,10 +2534,10 @@
       <c r="H10" s="3" t="s">
         <v>242</v>
       </c>
-      <c r="I10" s="7" t="s">
+      <c r="I10" s="6" t="s">
         <v>239</v>
       </c>
-      <c r="J10" s="7" t="s">
+      <c r="J10" s="6" t="s">
         <v>240</v>
       </c>
       <c r="Q10" s="2"/>
@@ -2442,10 +2568,10 @@
       <c r="H11" s="3" t="s">
         <v>244</v>
       </c>
-      <c r="I11" s="7" t="s">
+      <c r="I11" s="6" t="s">
         <v>241</v>
       </c>
-      <c r="J11" s="7" t="s">
+      <c r="J11" s="6" t="s">
         <v>242</v>
       </c>
       <c r="Q11" s="2"/>
@@ -2476,10 +2602,10 @@
       <c r="H12" s="3" t="s">
         <v>246</v>
       </c>
-      <c r="I12" s="7" t="s">
+      <c r="I12" s="6" t="s">
         <v>243</v>
       </c>
-      <c r="J12" s="7" t="s">
+      <c r="J12" s="6" t="s">
         <v>244</v>
       </c>
       <c r="Q12" s="2"/>
@@ -2510,10 +2636,10 @@
       <c r="H13" t="s">
         <v>222</v>
       </c>
-      <c r="I13" s="7" t="s">
+      <c r="I13" s="6" t="s">
         <v>245</v>
       </c>
-      <c r="J13" s="7" t="s">
+      <c r="J13" s="6" t="s">
         <v>246</v>
       </c>
       <c r="Q13" s="2"/>
@@ -2816,10 +2942,10 @@
       <c r="H22" s="3" t="s">
         <v>262</v>
       </c>
-      <c r="I22" s="7" t="s">
+      <c r="I22" s="6" t="s">
         <v>259</v>
       </c>
-      <c r="J22" s="7" t="s">
+      <c r="J22" s="6" t="s">
         <v>260</v>
       </c>
       <c r="Q22" s="2"/>
@@ -2884,10 +3010,10 @@
       <c r="H24" t="s">
         <v>265</v>
       </c>
-      <c r="I24" s="7" t="s">
+      <c r="I24" s="6" t="s">
         <v>263</v>
       </c>
-      <c r="J24" s="7" t="s">
+      <c r="J24" s="6" t="s">
         <v>226</v>
       </c>
       <c r="Q24" s="2"/>
@@ -3433,10 +3559,10 @@
       </c>
       <c r="E43" s="1"/>
       <c r="F43" s="1"/>
-      <c r="G43" s="8" t="s">
+      <c r="G43" t="s">
         <v>300</v>
       </c>
-      <c r="H43" s="8" t="s">
+      <c r="H43" t="s">
         <v>301</v>
       </c>
       <c r="I43" s="3" t="s">
@@ -3467,10 +3593,10 @@
       <c r="H44" s="3" t="s">
         <v>303</v>
       </c>
-      <c r="I44" s="8" t="s">
+      <c r="I44" t="s">
         <v>300</v>
       </c>
-      <c r="J44" s="8" t="s">
+      <c r="J44" t="s">
         <v>525</v>
       </c>
     </row>
@@ -3545,10 +3671,10 @@
       </c>
       <c r="E47" s="1"/>
       <c r="F47" s="1"/>
-      <c r="G47" s="8" t="s">
+      <c r="G47" t="s">
         <v>308</v>
       </c>
-      <c r="H47" s="8" t="s">
+      <c r="H47" t="s">
         <v>309</v>
       </c>
       <c r="I47" s="3" t="s">
@@ -3573,16 +3699,16 @@
       </c>
       <c r="E48" s="1"/>
       <c r="F48" s="1"/>
-      <c r="G48" s="8" t="s">
+      <c r="G48" t="s">
         <v>310</v>
       </c>
-      <c r="H48" s="8" t="s">
+      <c r="H48" t="s">
         <v>309</v>
       </c>
-      <c r="I48" s="8" t="s">
+      <c r="I48" t="s">
         <v>308</v>
       </c>
-      <c r="J48" s="8" t="s">
+      <c r="J48" t="s">
         <v>309</v>
       </c>
     </row>
@@ -3601,16 +3727,16 @@
       </c>
       <c r="E49" s="1"/>
       <c r="F49" s="1"/>
-      <c r="G49" s="8" t="s">
+      <c r="G49" t="s">
         <v>311</v>
       </c>
-      <c r="H49" s="8" t="s">
+      <c r="H49" t="s">
         <v>309</v>
       </c>
-      <c r="I49" s="8" t="s">
+      <c r="I49" t="s">
         <v>310</v>
       </c>
-      <c r="J49" s="8" t="s">
+      <c r="J49" t="s">
         <v>309</v>
       </c>
     </row>
@@ -3635,10 +3761,10 @@
       <c r="H50" s="3" t="s">
         <v>313</v>
       </c>
-      <c r="I50" s="8" t="s">
+      <c r="I50" t="s">
         <v>311</v>
       </c>
-      <c r="J50" s="8" t="s">
+      <c r="J50" t="s">
         <v>309</v>
       </c>
     </row>
@@ -3677,10 +3803,10 @@
       <c r="B52" t="s">
         <v>102</v>
       </c>
-      <c r="G52" s="8" t="s">
+      <c r="G52" t="s">
         <v>316</v>
       </c>
-      <c r="H52" s="8" t="s">
+      <c r="H52" t="s">
         <v>317</v>
       </c>
       <c r="I52" s="3" t="s">
@@ -3703,10 +3829,10 @@
       <c r="H53" t="s">
         <v>319</v>
       </c>
-      <c r="I53" s="8" t="s">
+      <c r="I53" t="s">
         <v>316</v>
       </c>
-      <c r="J53" s="8" t="s">
+      <c r="J53" t="s">
         <v>317</v>
       </c>
     </row>
@@ -3823,10 +3949,10 @@
       <c r="H59" s="3" t="s">
         <v>331</v>
       </c>
-      <c r="I59" s="7" t="s">
+      <c r="I59" s="6" t="s">
         <v>326</v>
       </c>
-      <c r="J59" s="7" t="s">
+      <c r="J59" s="6" t="s">
         <v>327</v>
       </c>
     </row>
@@ -4648,7 +4774,240 @@
 </worksheet>
 </file>
 
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7F997DDC-A27B-9E4F-9FC9-66FC153579BE}">
+  <dimension ref="A1:C28"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C7" sqref="C7"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="39.33203125" customWidth="1"/>
+    <col min="3" max="3" width="36" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:3" ht="17" x14ac:dyDescent="0.2">
+      <c r="A1" s="8" t="s">
+        <v>547</v>
+      </c>
+      <c r="C1" s="8" t="s">
+        <v>556</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" ht="17" x14ac:dyDescent="0.2">
+      <c r="A2" s="9" t="s">
+        <v>548</v>
+      </c>
+      <c r="C2" s="9" t="s">
+        <v>554</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" ht="17" x14ac:dyDescent="0.2">
+      <c r="A3" s="9" t="s">
+        <v>549</v>
+      </c>
+      <c r="C3" s="9" t="s">
+        <v>555</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" ht="17" x14ac:dyDescent="0.2">
+      <c r="A4" s="9" t="s">
+        <v>550</v>
+      </c>
+      <c r="C4" s="9" t="s">
+        <v>550</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" ht="17" x14ac:dyDescent="0.2">
+      <c r="A5" s="9" t="s">
+        <v>551</v>
+      </c>
+      <c r="C5" s="9" t="s">
+        <v>551</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" ht="17" x14ac:dyDescent="0.2">
+      <c r="A6" s="9" t="s">
+        <v>552</v>
+      </c>
+      <c r="C6" s="9" t="s">
+        <v>552</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3" ht="17" x14ac:dyDescent="0.2">
+      <c r="A7" s="10" t="s">
+        <v>553</v>
+      </c>
+      <c r="C7" s="10" t="s">
+        <v>553</v>
+      </c>
+    </row>
+    <row r="9" spans="1:3" ht="34" x14ac:dyDescent="0.2">
+      <c r="A9" s="12" t="s">
+        <v>557</v>
+      </c>
+      <c r="C9" s="11"/>
+    </row>
+    <row r="10" spans="1:3" ht="34" x14ac:dyDescent="0.2">
+      <c r="A10" s="10" t="s">
+        <v>558</v>
+      </c>
+      <c r="C10" s="10" t="s">
+        <v>558</v>
+      </c>
+    </row>
+    <row r="11" spans="1:3" ht="34" x14ac:dyDescent="0.2">
+      <c r="A11" s="10" t="s">
+        <v>559</v>
+      </c>
+      <c r="C11" s="10" t="s">
+        <v>559</v>
+      </c>
+    </row>
+    <row r="12" spans="1:3" ht="34" x14ac:dyDescent="0.2">
+      <c r="A12" s="10" t="s">
+        <v>560</v>
+      </c>
+      <c r="C12" s="10" t="s">
+        <v>560</v>
+      </c>
+    </row>
+    <row r="13" spans="1:3" ht="34" x14ac:dyDescent="0.2">
+      <c r="A13" s="10" t="s">
+        <v>561</v>
+      </c>
+      <c r="C13" s="10" t="s">
+        <v>561</v>
+      </c>
+    </row>
+    <row r="14" spans="1:3" ht="17" x14ac:dyDescent="0.2">
+      <c r="A14" s="10" t="s">
+        <v>562</v>
+      </c>
+      <c r="C14" s="10" t="s">
+        <v>562</v>
+      </c>
+    </row>
+    <row r="15" spans="1:3" ht="17" x14ac:dyDescent="0.2">
+      <c r="A15" s="10" t="s">
+        <v>563</v>
+      </c>
+      <c r="C15" s="10" t="s">
+        <v>563</v>
+      </c>
+    </row>
+    <row r="16" spans="1:3" ht="17" x14ac:dyDescent="0.2">
+      <c r="A16" s="10" t="s">
+        <v>564</v>
+      </c>
+      <c r="C16" s="10" t="s">
+        <v>564</v>
+      </c>
+    </row>
+    <row r="17" spans="1:3" ht="17" x14ac:dyDescent="0.2">
+      <c r="A17" s="10" t="s">
+        <v>565</v>
+      </c>
+      <c r="C17" s="10" t="s">
+        <v>565</v>
+      </c>
+    </row>
+    <row r="18" spans="1:3" ht="34" x14ac:dyDescent="0.2">
+      <c r="A18" s="10" t="s">
+        <v>566</v>
+      </c>
+      <c r="C18" s="12" t="s">
+        <v>567</v>
+      </c>
+    </row>
+    <row r="20" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A20" s="11" t="s">
+        <v>568</v>
+      </c>
+      <c r="C20" s="11" t="s">
+        <v>568</v>
+      </c>
+    </row>
+    <row r="21" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A21" s="11" t="s">
+        <v>569</v>
+      </c>
+      <c r="C21" s="11" t="s">
+        <v>569</v>
+      </c>
+    </row>
+    <row r="22" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A22" s="11" t="s">
+        <v>570</v>
+      </c>
+      <c r="C22" s="11" t="s">
+        <v>570</v>
+      </c>
+    </row>
+    <row r="23" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A23" s="11" t="s">
+        <v>571</v>
+      </c>
+      <c r="C23" s="11" t="s">
+        <v>571</v>
+      </c>
+    </row>
+    <row r="24" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A24" s="11" t="s">
+        <v>572</v>
+      </c>
+      <c r="C24" s="11" t="s">
+        <v>572</v>
+      </c>
+    </row>
+    <row r="25" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A25" s="11" t="s">
+        <v>573</v>
+      </c>
+      <c r="C25" s="11" t="s">
+        <v>573</v>
+      </c>
+    </row>
+    <row r="26" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A26" s="11" t="s">
+        <v>574</v>
+      </c>
+      <c r="C26" s="11" t="s">
+        <v>574</v>
+      </c>
+    </row>
+    <row r="27" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A27" s="11" t="s">
+        <v>575</v>
+      </c>
+      <c r="C27" s="11" t="s">
+        <v>575</v>
+      </c>
+    </row>
+    <row r="28" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A28" s="13" t="s">
+        <v>576</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <TaxCatchAll xmlns="d391a701-1e72-4a9c-8e27-32ae852ac85b" xsi:nil="true"/>
+    <lcf76f155ced4ddcb4097134ff3c332f xmlns="748de206-7911-403a-93a2-ff3feb5ad88e">
+      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    </lcf76f155ced4ddcb4097134ff3c332f>
+  </documentManagement>
+</p:properties>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x0101009FE99232C2A610489C05CA2A95C6B0DC" ma:contentTypeVersion="16" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="99e3d855f4612a477f80c26c84225e60">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="748de206-7911-403a-93a2-ff3feb5ad88e" xmlns:ns3="d391a701-1e72-4a9c-8e27-32ae852ac85b" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="9d24ec2972380c9becf470258562e41c" ns2:_="" ns3:_="">
     <xsd:import namespace="748de206-7911-403a-93a2-ff3feb5ad88e"/>
@@ -4879,17 +5238,6 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <TaxCatchAll xmlns="d391a701-1e72-4a9c-8e27-32ae852ac85b" xsi:nil="true"/>
-    <lcf76f155ced4ddcb4097134ff3c332f xmlns="748de206-7911-403a-93a2-ff3feb5ad88e">
-      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    </lcf76f155ced4ddcb4097134ff3c332f>
-  </documentManagement>
-</p:properties>
-</file>
-
 <file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <?mso-contentType ?>
 <FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
@@ -4900,6 +5248,23 @@
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{8A0F7ED7-B064-47CF-BC44-4A045BE18651}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="748de206-7911-403a-93a2-ff3feb5ad88e"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="d391a701-1e72-4a9c-8e27-32ae852ac85b"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{425960D1-4FA0-44B7-8D5C-E9238875A675}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -4918,23 +5283,6 @@
 </ds:datastoreItem>
 </file>
 
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{8A0F7ED7-B064-47CF-BC44-4A045BE18651}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="d391a701-1e72-4a9c-8e27-32ae852ac85b"/>
-    <ds:schemaRef ds:uri="748de206-7911-403a-93a2-ff3feb5ad88e"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{FBF3EE50-7D40-453B-9B2A-4D1C4E8CD157}">
   <ds:schemaRefs>

</xml_diff>